<commit_message>
updating sample files and docs
</commit_message>
<xml_diff>
--- a/sample_documents/Azure Search Pricing Table.xlsx
+++ b/sample_documents/Azure Search Pricing Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/chromer_microsoft_com1/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delegenz\Source\azure-search-knowledge-mining\sample_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{1AD10545-5259-4A9C-A139-17C14520001F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{50C16610-F163-4386-B0F0-AABE6827B163}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050DE06B-B5E9-4388-AEBC-8158D424FAD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A39AA46E-378E-4E67-B25B-F39D55F25457}"/>
   </bookViews>
@@ -231,7 +231,7 @@
     <t>$3.839/hour</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: This data was taken on 6/12/2019 from https://azure.microsoft.com/en-us/pricing/details/search/ </t>
+    <t>Note: This data was taken on 6/12/2019. Please see https://azure.microsoft.com/en-us/pricing/details/search/ for up to date pricing</t>
   </si>
 </sst>
 </file>
@@ -355,19 +355,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,7 +686,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -742,9 +742,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="25.9" x14ac:dyDescent="0.45">
-      <c r="A3" s="7"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
@@ -788,10 +788,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -814,8 +814,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
@@ -836,8 +836,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.9" x14ac:dyDescent="0.45">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -850,7 +850,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -876,7 +876,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.9" x14ac:dyDescent="0.45">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="7"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>34</v>
@@ -922,7 +922,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>35</v>
@@ -973,16 +973,16 @@
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A8:A11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>